<commit_message>
galacticPubs::publish() [2022-06-30 11:50:01]  update QuickPrep for all lessons
</commit_message>
<xml_diff>
--- a/meta/procedure_GSheetsOnly.xlsx
+++ b/meta/procedure_GSheetsOnly.xlsx
@@ -259,13 +259,13 @@
     <t>Start by figuring out how many dye colours we brought with us today. Using a worksheet, students calculate their "dye-versity index".</t>
   </si>
   <si>
-    <t xml:space="preserve">Using a worksheet, students calculate their "dye-versity index". This number represents the total number of colours a student has on them, and therefore the number of dye processes that had to be invented. </t>
+    <t xml:space="preserve">The "dye-versity index" represents the total number of colours a student has on them, and therefore the number of dye processes that had to be invented. </t>
   </si>
   <si>
     <t>Share Out</t>
   </si>
   <si>
-    <t>Students share their "dye-versity index" and reflect on whether colour helps express their personality or mood. They will also begin to think about natural vs dyed colours.</t>
+    <t>Students share their "dye-versity index" and reflect on whether colour helps express their personality or mood.</t>
   </si>
   <si>
     <t>Chunks: 4
@@ -370,7 +370,8 @@
     <t>Activity instructions</t>
   </si>
   <si>
-    <t xml:space="preserve">To help students think about initial costs of each dye technology, they are given a set of Cost Cards {item2} with the steps of each process. </t>
+    <t xml:space="preserve">{item2}  
+To help students think about initial costs of each dye technology, they are given a set of Cost Cards with the steps of each process. </t>
   </si>
   <si>
     <t>Each group of students will receive a set of 18 Cost Cards that contain the steps in each of the three dyeing technologies (six steps per process). The presentation will break the activity into substages and guide the students through an analysis of the processes.
@@ -412,7 +413,7 @@
     <t>Introducing Price Curves</t>
   </si>
   <si>
-    <t>The presentation guides the introduction of producing items at various scales and discusses how the price per unit changes accordingly.</t>
+    <t>The presentation introduces the idea of producing items at various scales and discusses how the price per unit changes accordingly.</t>
   </si>
   <si>
     <t xml:space="preserve">Students use their worksheets to follow the discussion of Price Curves and answer questions throughout the presentation. </t>
@@ -424,10 +425,10 @@
     <t>The example of fishing for Murex snails illustrates how the availability of resources affects (and limits) the scale of production.</t>
   </si>
   <si>
-    <t>Watch True Blues: Textiles Water Pollution Problem {vid3} to learn about some of the environmental impacts of synthetic dyes made from fossil fuels.</t>
+    <t>{vid3} Learn about some of the environmental impacts of synthetic dyes made from fossil fuels.</t>
   </si>
   <si>
-    <t>Throughout the presentation, synthetic dyes produced from fossil fuels become an increasingly attractive dye technology. Despite their range of colours and low costs, dyes produced from fossil fuels also cause a lot of problems. In this video students learn about the many sustainability issues tied to the dye and fashion industries (particularly with fossil-fuel-derived synthetic dyes). This prepares students to reflect on and analyse the consequences of dye technologies as they perform a cost-benefit analysis of the available dye technologies to make a recommendation for *Galactic Tees*.</t>
+    <t>Throughout the presentation, synthetic dyes produced from fossil fuels are shown to be a competitive and attractive dye technology. Despite their range of colours and low costs, dyes produced from fossil fuels also cause a lot of problems. In this video students learn about the many sustainability issues tied to the dye and fashion industries (particularly with fossil-fuel-derived synthetic dyes). This prepares students to reflect on and analyse the consequences of dye technologies as they perform a cost-benefit analysis of the available dye technologies to make a recommendation for *Galactic Tees*.</t>
   </si>
   <si>
     <t>Interpretation and Reflection</t>

</xml_diff>